<commit_message>
Bug fix log manager and others
- bug fix log manager: records now human moves as well in the log
- simplified TDNTuple2Agt: commented unnecessary code out, may be
deleted later
- bug fix for restoring older agents which had no ParOther m_oPar in the
saved version (setDefaultOtherPar() added)
- extended evaluator mode 10 for Hex (see HexConfig#EVAL_START_ACTIONS)
- bugFix: serialVersionUID for classes implementing interface
XNTupleFuncs
- small docu changes
</commit_message>
<xml_diff>
--- a/agents/2048/fixed 4 6-Tupels 100k TDNT2 afterState.xlsx
+++ b/agents/2048/fixed 4 6-Tupels 100k TDNT2 afterState.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7068"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7068" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>&lt; 1024</t>
   </si>
@@ -417,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -619,4 +620,212 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <f>SUM(D6:G6)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
+        <f>H6/H$11</f>
+        <v>0.01</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ref="J6:J8" si="0">J7+I6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1024</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H10" si="1">SUM(D7:G7)</f>
+        <v>9</v>
+      </c>
+      <c r="I7" s="4">
+        <f>H7/H$11</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.9900000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>2048</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I8" s="4">
+        <f>H8/H$11</f>
+        <v>0.19</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.94500000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>4096</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>31</v>
+      </c>
+      <c r="G9">
+        <v>22</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I9" s="4">
+        <f>H9/H$11</f>
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="5">
+        <f>J10+I9</f>
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D10" s="1">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="I10" s="6">
+        <f>H10/H$11</f>
+        <v>0.255</v>
+      </c>
+      <c r="J10" s="7">
+        <f>I10</f>
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f>SUM(D6:D10)</f>
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:H11" si="2">SUM(E6:E10)</f>
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NEW_3P and other changes
This large commit contains a number of changes
- NEW_3P: a switch in TDNTuple2Agt for a new TD update scheme which
works for 1-,2-,3-,... player games consistently
- new functions StateObservation::getReward to allow another reward than
game score
- switch OtherParams,ParOther::rewardIsGameScore to select between two
different rewards (currently only effective for 2048: cumulative empty
tiles)
- GameBoard::showGameBoard with a new option alignToMain
- new functions in StateObservation: advanceDeterministic,
advanceNondeterministic, getPrecedingAfterstate to make TD algorithms
generic for all cases
- many new multiTrain csv files
- all associated R plot files (multiTrain, playStats) moved to
resources/R_plotTools
</commit_message>
<xml_diff>
--- a/agents/2048/fixed 4 6-Tupels 100k TDNT2 afterState.xlsx
+++ b/agents/2048/fixed 4 6-Tupels 100k TDNT2 afterState.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t>&lt; 1024</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>percent cum</t>
+  </si>
+  <si>
+    <t>fixed 4 6-Tupels 200k TDNT2 afterState.agt.zip</t>
+  </si>
+  <si>
+    <t>fixed TEST eTiles 4 6-Tupels 200k TDNT2 afterState.agt.zip</t>
   </si>
 </sst>
 </file>
@@ -624,10 +630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J11"/>
+  <dimension ref="B2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,6 +830,390 @@
         <v>200</v>
       </c>
     </row>
+    <row r="14" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f>SUM(D18:G18)</f>
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
+        <f>H18/H$11</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" ref="J18:J20" si="3">J19+I18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>1024</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" ref="H19:H22" si="4">SUM(D19:G19)</f>
+        <v>8</v>
+      </c>
+      <c r="I19" s="4">
+        <f>H19/H$11</f>
+        <v>0.04</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="3"/>
+        <v>0.97500000000000009</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>2048</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="I20" s="4">
+        <f>H20/H$11</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="3"/>
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>4096</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>27</v>
+      </c>
+      <c r="F21">
+        <v>23</v>
+      </c>
+      <c r="G21">
+        <v>13</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="I21" s="4">
+        <f>H21/H$11</f>
+        <v>0.4</v>
+      </c>
+      <c r="J21" s="5">
+        <f>J22+I21</f>
+        <v>0.86499999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D22" s="1">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16</v>
+      </c>
+      <c r="F22" s="1">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1">
+        <v>31</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="I22" s="6">
+        <f>H22/H$11</f>
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="J22" s="7">
+        <f>I22</f>
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <f>SUM(D18:D22)</f>
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:H23" si="5">SUM(E18:E22)</f>
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <f>SUM(D30:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <f>H30/H$11</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" ref="J30:J32" si="6">J31+I30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>1024</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" ref="H31:H34" si="7">SUM(D31:G31)</f>
+        <v>3</v>
+      </c>
+      <c r="I31" s="4">
+        <f>H31/H$11</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>2048</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="I32" s="4">
+        <f>H32/H$11</f>
+        <v>0.05</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="6"/>
+        <v>0.9850000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>4096</v>
+      </c>
+      <c r="D33">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <v>27</v>
+      </c>
+      <c r="F33">
+        <v>19</v>
+      </c>
+      <c r="G33">
+        <v>26</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="7"/>
+        <v>92</v>
+      </c>
+      <c r="I33" s="4">
+        <f>H33/H$11</f>
+        <v>0.46</v>
+      </c>
+      <c r="J33" s="5">
+        <f>J34+I33</f>
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C34" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D34" s="1">
+        <v>24</v>
+      </c>
+      <c r="E34" s="1">
+        <v>21</v>
+      </c>
+      <c r="F34" s="1">
+        <v>27</v>
+      </c>
+      <c r="G34" s="1">
+        <v>23</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="I34" s="6">
+        <f>H34/H$11</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="J34" s="7">
+        <f>I34</f>
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <f>SUM(D30:D34)</f>
+        <v>50</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ref="E35:H35" si="8">SUM(E30:E34)</f>
+        <v>50</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="8"/>
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>